<commit_message>
Peticiones a academia casi concluidas
</commit_message>
<xml_diff>
--- a/Xlsx Pruebas/ListaProfesores/ProfesInformatica.xlsx
+++ b/Xlsx Pruebas/ListaProfesores/ProfesInformatica.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19330"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A78F7A0D-739C-41E9-B013-80E01165F9EA}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C9C8CA3-DC44-4117-A0C9-69EEC1C17ACA}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -28,9 +28,6 @@
     <t>Apellidos</t>
   </si>
   <si>
-    <t>No. Nómina</t>
-  </si>
-  <si>
     <t>Ismael</t>
   </si>
   <si>
@@ -43,10 +40,13 @@
     <t>Luis René</t>
   </si>
   <si>
-    <t>Nombre(s)</t>
-  </si>
-  <si>
     <t>Durán Hernández</t>
+  </si>
+  <si>
+    <t>NumNomina</t>
+  </si>
+  <si>
+    <t>Nombres</t>
   </si>
 </sst>
 </file>
@@ -377,28 +377,28 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.20703125" customWidth="1"/>
-    <col min="2" max="2" width="20.734375" customWidth="1"/>
-    <col min="3" max="3" width="25.41796875" customWidth="1"/>
+    <col min="1" max="1" width="16.140625" customWidth="1"/>
+    <col min="2" max="2" width="20.7109375" customWidth="1"/>
+    <col min="3" max="3" width="25.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="B1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>12</v>
       </c>
@@ -406,32 +406,32 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>13</v>
       </c>
       <c r="B3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
         <v>3</v>
       </c>
-      <c r="C3" t="s">
-        <v>4</v>
-      </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>14</v>
       </c>
       <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
         <v>6</v>
       </c>
-      <c r="C4" t="s">
-        <v>8</v>
-      </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C8" s="2"/>
     </row>
   </sheetData>

</xml_diff>